<commit_message>
added a new method: whatWasSent
</commit_message>
<xml_diff>
--- a/xlsx/rasp.xlsx
+++ b/xlsx/rasp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
   <si>
     <t>Напоминание к занятию 4.2.</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>SEO-13/123</t>
-  </si>
-  <si>
-    <t>PHP-9/321</t>
   </si>
   <si>
     <t>Событие</t>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>Пароль группы</t>
+  </si>
+  <si>
+    <t>DS-1/offline</t>
   </si>
 </sst>
 </file>
@@ -452,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,173 +468,227 @@
   <sheetData>
     <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B2" s="5">
-        <v>42958.71875</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="7"/>
+        <v>42972.989583333336</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>5</v>
+      <c r="A3" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B3" s="5">
-        <v>42959.1875</v>
+        <v>42972.864583333336</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5">
+        <v>42972.854166666664</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="5">
-        <v>42936.708333333336</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5">
+        <v>42972.833333333336</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="5">
-        <v>42941.708333333336</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B6" s="5">
-        <v>42948.052083333336</v>
+        <v>42973.020833333336</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>8</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5">
-        <v>42936.708333333336</v>
+        <v>42973.03125</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>9</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B8" s="5">
-        <v>42958.71875</v>
+        <v>42973.041666666664</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5">
+        <v>42973.364583333336</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5">
+        <v>42973.729166666664</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5">
+        <v>42973.895833333336</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-    </row>
-    <row r="16" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+    <row r="12" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5">
+        <v>42973.90625</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5">
+        <v>42973.916666666664</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="5">
+        <v>42973.927083333336</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="5">
+        <v>42973.9375</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="5">
+        <v>42973.947916666664</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5">
+        <v>42973.916666666664</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
@@ -678,6 +732,60 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
     </row>
+    <row r="26" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added a web eldule list
</commit_message>
<xml_diff>
--- a/xlsx/rasp.xlsx
+++ b/xlsx/rasp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="36">
   <si>
     <t>Напоминание к занятию 4.2.</t>
   </si>
@@ -80,6 +80,76 @@
   </si>
   <si>
     <t>DS-1/offline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Внимание!* Сегодня занятия не будет. Вынуждены перенести его на среду в то же время. 
+Простите нас.
+</t>
+  </si>
+  <si>
+    <t>Добрый день! Anaconda, matplotlib, ноутбук — вот что нужно сегодня взять на занятие. До встречи!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Доброе утро. 
+Занятие по основам нейросетей будет в малой аудитории «Ключа», а не в большой. Начинаем через 15 минут.  </t>
+  </si>
+  <si>
+    <t>Добрый день. Сегодня в 19:00 будет занятие по основам нейросетей. Место — стеклянная аудитория «Ключа».</t>
+  </si>
+  <si>
+    <t>Доброе утро. На всякий случай напоминаем, что сегодня занятия нет: каникулы же. Отличного отдыха!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Перед занятием Славы советую пройти [вот этот](yandex.ru) классный курс по нейросетям. </t>
+  </si>
+  <si>
+    <t>Занятие начнётся чуть позже: преподаватель в пробке. Если ещё не на месте, можете сбавить ход и отдышаться.</t>
+  </si>
+  <si>
+    <t>ADM-1/offline</t>
+  </si>
+  <si>
+    <t>ADM-2/offline</t>
+  </si>
+  <si>
+    <t>Доброе утро.
+Занятие «Как быть Зеной — королевой войнов и не облажаться» начнётся через 15 минут. Место — Амфиполис. На проходной нужно сказать, что в «Нетологию».</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый день.
+Сегодня в 19:00 будет занятие «Твиттер для пожилых кондукторов: возможности, вызовы». С собой нужен будет ноутбук. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый день!
+Сегодня в 19:00 будет занятие «Как вести Инстаграм, если ты — булочка с корицей». Проведёт Екатерина Пушкарёва.
+*Важно* Напоминаем, что с собой нужно взять документы, чтобы потом вам оформить и выдать диплом:
+− паспорт;
+− билет банка приколов;
+− дисперсию.
+</t>
+  </si>
+  <si>
+    <t>Добрый день!
+Сегодня в 19:00 будет занятие «Как вести Инстаграм, если ты — булочка с корицей». Проведёт Екатерина Пушкарёва.
+*Важно* Напоминаем, что с собой нужно взять документы, чтобы потом вам оформить и выдать диплом:
+− паспорт;
+− билет банка приколов;
+− дисперсию.</t>
+  </si>
+  <si>
+    <t>Привет, Андрей!
+Напоминаем, планёрка начнётся через 15 минут в стеклянной переговорке. Будем обсуждать методичку Кампуса. Не опаздывай.</t>
+  </si>
+  <si>
+    <t>Привет, Наташа! 
+Напоминаем, планёрка начнётся через 15 минут в стеклянной переговорке. Будем обсуждать методичку Кампуса. Не опаздывай.</t>
+  </si>
+  <si>
+    <t>Привет, Оля! 
+Напоминаем, планёрка начнётся через 15 минут в стеклянной переговорке. Будем обсуждать методичку Кампуса. Не опаздывай.</t>
+  </si>
+  <si>
+    <t>PHP-9/123</t>
   </si>
 </sst>
 </file>
@@ -118,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -148,6 +218,16 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -452,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +543,7 @@
     <col min="1" max="1" width="21.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="104.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="56.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="56.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -485,306 +565,595 @@
         <v>18</v>
       </c>
       <c r="B2" s="5">
-        <v>42972.989583333336</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
-        <v>16</v>
-      </c>
+        <v>42982.666666666664</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B3" s="5">
-        <v>42972.864583333336</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="6"/>
+        <v>42982.666666666664</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B4" s="5">
-        <v>42972.854166666664</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="6"/>
+        <v>42982.666666666664</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="5">
-        <v>42972.833333333336</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="6"/>
+        <v>42980.4375</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B6" s="5">
-        <v>42973.020833333336</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="6"/>
+        <v>42980.4375</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5">
+        <v>42980.4375</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="5">
+        <v>42979.791666666664</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5">
+        <v>42979.791666666664</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5">
+        <v>42979.791666666664</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="5">
+        <v>42979.78125</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="5">
+        <v>42979.78125</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5">
+        <v>42979.78125</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="5">
+        <v>42978.78125</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="5">
+        <v>42978.78125</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="5">
+        <v>42978.78125</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="5">
+        <v>42978.770833333336</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5">
+        <v>42978.770833333336</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5">
+        <v>42978.770833333336</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5">
+        <v>42978.4375</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="5">
+        <v>42977.791666666664</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="5">
+        <v>42977.708333333336</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="5">
+        <v>42977.625</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="5">
+        <v>42977.4375</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="5">
+        <v>42976.895833333336</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="5">
+        <v>42976.864583333336</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="5">
+        <v>42972.989583333336</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="5">
+        <v>42972.864583333336</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="5">
+        <v>42972.854166666664</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="5">
+        <v>42972.833333333336</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="5">
+        <v>42973.020833333336</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="5">
         <v>42973.03125</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="5">
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="5">
         <v>42973.041666666664</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="5">
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="5">
         <v>42973.364583333336</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="5">
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="5">
         <v>42973.729166666664</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:4" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="D35" s="9"/>
+    </row>
+    <row r="36" spans="1:4" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B36" s="5">
         <v>42973.895833333336</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B37" s="5">
         <v>42973.90625</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D37" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="5">
+    <row r="38" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="5">
+        <v>42979.177083333336</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="5">
+        <v>42979.1875</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="5">
+        <v>42973.9375</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="5">
+        <v>42973.947916666664</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="5">
         <v>42973.916666666664</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="5">
-        <v>42973.927083333336</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="5">
-        <v>42973.9375</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="5">
-        <v>42973.947916666664</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="5">
-        <v>42973.916666666664</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D42" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-    </row>
-    <row r="24" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-    </row>
-    <row r="32" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-    </row>
-    <row r="33" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
+    <row r="43" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+    </row>
+    <row r="48" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="5"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="5"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="5"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="5"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="5"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>